<commit_message>
Cambios en lectura de excel
Cambios en la lectura del excel + incorporación de algunos test
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -3,18 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\cursos\asw\LoadUsers\src\test\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8370" windowHeight="2370"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10545" windowHeight="2130"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Nombre</t>
   </si>
@@ -32,9 +28,6 @@
     <t>Colegio</t>
   </si>
   <si>
-    <t>Mesa</t>
-  </si>
-  <si>
     <t>NIF</t>
   </si>
   <si>
@@ -54,16 +47,36 @@
   </si>
   <si>
     <t>09940449X</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>juantp@gmail.com</t>
+  </si>
+  <si>
+    <t>luislf@gmail.com</t>
+  </si>
+  <si>
+    <t>anatp@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -86,14 +99,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -375,7 +391,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -388,59 +404,64 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2">
         <v>234</v>
       </c>
-      <c r="D2">
-        <v>2</v>
+      <c r="D2" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
       </c>
       <c r="C3">
         <v>345</v>
       </c>
-      <c r="D3">
-        <v>2</v>
+      <c r="D3" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="C4">
         <v>456</v>
       </c>
-      <c r="D4">
-        <v>3</v>
+      <c r="D4" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="D4" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>